<commit_message>
sketch and signature finalized
</commit_message>
<xml_diff>
--- a/app/config/tables/imageSubform/forms/imageSubform/imageSubform.xlsx
+++ b/app/config/tables/imageSubform/forms/imageSubform/imageSubform.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>clause</t>
   </si>
@@ -82,6 +82,12 @@
     <t>Photo</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Photo name</t>
+  </si>
+  <si>
     <t>textarea</t>
   </si>
   <si>
@@ -130,10 +136,10 @@
     <t>Image Subform</t>
   </si>
   <si>
+    <t>instance_name</t>
+  </si>
+  <si>
     <t>parent_id</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
 </sst>
 </file>
@@ -383,10 +389,10 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="5"/>
@@ -394,53 +400,76 @@
       <c r="L3" s="3"/>
       <c r="M3" s="7"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="P3" s="6">
-        <v>255.0</v>
-      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="5"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="M4" s="7"/>
       <c r="N4" s="3"/>
+      <c r="O4" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>255.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="M5" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="N5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -460,49 +489,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" s="11">
-        <v>2.0160101002E10</v>
+        <v>2.0160101003E10</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="C4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -530,16 +567,16 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>22</v>
@@ -548,27 +585,33 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="6">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="3"/>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
     </row>
     <row r="15">
       <c r="B15" s="3"/>
     </row>
-    <row r="18">
-      <c r="B18" s="3"/>
+    <row r="16">
+      <c r="B16" s="3"/>
     </row>
     <row r="19">
       <c r="B19" s="3"/>
@@ -577,13 +620,16 @@
       <c r="B20" s="3"/>
     </row>
     <row r="21">
-      <c r="B21" s="8"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22">
-      <c r="B22" s="4"/>
+      <c r="B22" s="8"/>
     </row>
     <row r="23">
       <c r="B23" s="4"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>